<commit_message>
- automatic mode for the upper delta axis limit sets also a reasonable step size for the axis ticks - updated Giesen WxA+ machine setups - improved S7 serial logging and communication error handling - adds "fetch full blocks" option to instruct the S7 and MODBUS optimizer fetch maximal register blocks from lowest to largest register number - adds Artisan Commands: popup(m[,t]), message(s), setCanvasColor(c), resetCanvasColor, button(e) with e = { START, CHARGE, DRY, FCs, FCe, SCs, SCe, DROP, COOL, OFF }, p-i-d(p,i,d), pidSV(v), pidRS(n), pidSource(n) - adds Qt base translations for Turkish, Dutch and Brazilian
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/eventsliders.xlsx
+++ b/doc/help_dialogs/Input_files/eventsliders.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="209">
   <si>
     <t xml:space="preserve">EVENT CUSTOM SLIDERS</t>
   </si>
@@ -498,6 +498,60 @@
   </si>
   <si>
     <t xml:space="preserve">sets PID mode to 0: manual, 1: RS, 2: background follow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p-i-d(&lt;p&gt;,&lt;i&gt;,&lt;d&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sets the p-i-d parameters of the PID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pidSV(&lt;float&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sets the PID target set value SV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pidRS(&lt;int&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">activates the PID Ramp-Soak pattern number &lt;n&gt; (1-based!)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pidSource(&lt;int&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">selects the PID input source with &lt;n&gt; 0: BT, 1: ET (Software PID); &lt;n&gt; in {0,..,3} (Arduino PID)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">popup(&lt;msg&gt;[,&lt;int&gt;])</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shows popup with message &lt;msg&gt; which optionally automatically closes after &lt;int&gt; seconds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">message(&lt;msg&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shows message &lt;msg&gt; in the message line</t>
+  </si>
+  <si>
+    <t xml:space="preserve">setCanvasColor(&lt;color&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sets canvas color to the RGB-hex &lt;color&gt; like #27f1d3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">resetCanvasColor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">resets canvas color</t>
+  </si>
+  <si>
+    <t xml:space="preserve">button(&lt;name&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">activates button &lt;name&gt; from { START, CHARGE, DRY, FCs, FCe, SCs, SCe, DROP, COOL, OFF } </t>
   </si>
   <si>
     <t xml:space="preserve">playbackmode(&lt;int&gt;)</t>
@@ -702,10 +756,10 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="1" sqref="B35:B36 B6"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="1" sqref="B74:C82 B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="70.31"/>
@@ -820,13 +874,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C91"/>
+  <dimension ref="A1:C100"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A29" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B35" activeCellId="0" sqref="B35:B36"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A60" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B74" activeCellId="0" sqref="B74:C82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.57"/>
@@ -1441,7 +1495,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B74" s="0" t="s">
         <v>159</v>
       </c>
@@ -1449,7 +1503,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B75" s="0" t="s">
         <v>161</v>
       </c>
@@ -1457,138 +1511,210 @@
         <v>162</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="0" t="s">
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B76" s="0" t="s">
         <v>163</v>
       </c>
-      <c r="B76" s="0" t="s">
+      <c r="C76" s="0" t="s">
         <v>164</v>
       </c>
-      <c r="C76" s="0" t="s">
+    </row>
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B77" s="0" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B77" s="0" t="s">
+      <c r="C77" s="0" t="s">
         <v>166</v>
       </c>
-      <c r="C77" s="0" t="s">
+    </row>
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B78" s="0" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B78" s="0" t="s">
+      <c r="C78" s="0" t="s">
         <v>168</v>
       </c>
-      <c r="C78" s="0" t="s">
+    </row>
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B79" s="0" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B79" s="0" t="s">
+      <c r="C79" s="0" t="s">
         <v>170</v>
       </c>
-      <c r="C79" s="0" t="s">
+    </row>
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B80" s="0" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B80" s="0" t="s">
+      <c r="C80" s="0" t="s">
         <v>172</v>
       </c>
-      <c r="C80" s="0" t="s">
+    </row>
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B81" s="0" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B81" s="0" t="s">
+      <c r="C81" s="0" t="s">
         <v>174</v>
       </c>
-      <c r="C81" s="0" t="s">
+    </row>
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B82" s="0" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B82" s="0" t="s">
+      <c r="C82" s="0" t="s">
         <v>176</v>
-      </c>
-      <c r="C82" s="0" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B83" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="C83" s="0" t="s">
         <v>178</v>
-      </c>
-      <c r="C83" s="0" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B84" s="0" t="s">
-        <v>82</v>
+        <v>179</v>
       </c>
       <c r="C84" s="0" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="0" t="s">
+        <v>181</v>
+      </c>
       <c r="B85" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C85" s="0" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B86" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C86" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B87" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="C87" s="0" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B88" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="C88" s="0" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B89" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="C89" s="0" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B90" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="C90" s="0" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B91" s="0" t="s">
+        <v>194</v>
+      </c>
+      <c r="C91" s="0" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B92" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="C92" s="0" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B93" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C93" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B94" s="0" t="s">
+        <v>199</v>
+      </c>
+      <c r="C94" s="0" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B95" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="C95" s="0" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B96" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="C87" s="0" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="0" t="s">
-        <v>186</v>
-      </c>
-      <c r="B88" s="0" t="s">
-        <v>187</v>
-      </c>
-      <c r="C88" s="0" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B89" s="0" t="s">
+      <c r="C96" s="0" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="0" t="s">
+        <v>204</v>
+      </c>
+      <c r="B97" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="C97" s="0" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B98" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="C89" s="0" t="s">
+      <c r="C98" s="0" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B90" s="0" t="s">
+    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B99" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="C90" s="0" t="s">
+      <c r="C99" s="0" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B91" s="0" t="s">
-        <v>189</v>
-      </c>
-      <c r="C91" s="0" t="s">
-        <v>190</v>
+    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B100" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="C100" s="0" t="s">
+        <v>208</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- detects and adjusts to screen setup changes - adds Kaleido Network and Serial protocols and corresponding machine setups - fixes custom event button table drag-and-drop action - adds translated and state aware custom event button label tags - adds button action symbolic variable ^ bound to button state - adds additional Artisan Command, IO Command, MODBUS Command, S7 Command, WebSocket Command button actions to set button states - PIDon/PIDoff binds its new state to _ - updated help texts and translations
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/eventsliders.xlsx
+++ b/doc/help_dialogs/Input_files/eventsliders.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="271">
   <si>
     <t xml:space="preserve">EVENT CUSTOM SLIDERS</t>
   </si>
@@ -455,13 +455,37 @@
     <t xml:space="preserve">button(i,c,b[,sn])</t>
   </si>
   <si>
-    <t xml:space="preserve">switches channel c off (b=0) and on (b=1) and sets button i to pressed or normal depending on the value b</t>
+    <t xml:space="preserve">switches PHIDGET Binary Output channel c off (b=0) and on (b=1) and sets button i to pressed or normal depending on the value b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">button(i,b)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sets button i to pressed if value b is yes, true, t, or 1, otherwise to normal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">button(b)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sets button to pressed if value b is yes, true, t, or 1, otherwise to normal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">button()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toggles the state of the button</t>
   </si>
   <si>
     <t xml:space="preserve">santoker(&lt;target&gt;,&lt;value&gt;)</t>
   </si>
   <si>
     <t xml:space="preserve">sends integer &lt;value&gt; to &lt;target&gt; register specified by as byte in hex notation like “fa” via the Santoker Network protocol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kaleido(&lt;target&gt;,&lt;value&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sends &lt;value&gt; to &lt;target&gt; via the Kaleido Serial or Network protocol</t>
   </si>
   <si>
     <t xml:space="preserve">S7 Command</t>
@@ -934,10 +958,10 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="1" sqref="B65:C65 B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.94140625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="70.31"/>
@@ -1052,13 +1076,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C127"/>
+  <dimension ref="A1:C131"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J22" activeCellId="0" sqref="J22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A41" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B65" activeCellId="0" sqref="B65:C65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.94140625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.57"/>
@@ -1571,86 +1595,82 @@
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B63" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C63" s="0" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>145</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="2" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="1" t="s">
-        <v>147</v>
-      </c>
       <c r="B65" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
+      </c>
+      <c r="C65" s="0" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="1"/>
       <c r="B66" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C66" s="1" t="s">
+      <c r="C66" s="0" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="1"/>
       <c r="B67" s="2" t="s">
-        <v>36</v>
+        <v>151</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B68" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>151</v>
+        <v>153</v>
+      </c>
+      <c r="C68" s="0" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="1"/>
+      <c r="A69" s="1" t="s">
+        <v>155</v>
+      </c>
       <c r="B69" s="2" t="s">
-        <v>152</v>
+        <v>32</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1"/>
       <c r="B70" s="2" t="s">
-        <v>154</v>
+        <v>34</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>155</v>
+        <v>35</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1"/>
       <c r="B71" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="C71" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C71" s="0" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="1"/>
       <c r="B72" s="2" t="s">
         <v>158</v>
       </c>
@@ -1668,97 +1688,101 @@
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="0" t="s">
+      <c r="A74" s="1"/>
+      <c r="B74" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="B74" s="2"/>
-      <c r="C74" s="0" t="s">
+      <c r="C74" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="1"/>
+      <c r="B75" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="1"/>
+      <c r="B76" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="1"/>
+      <c r="B77" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="B78" s="2"/>
+      <c r="C78" s="0" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="B75" s="2"/>
-      <c r="C75" s="0" t="s">
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="B79" s="2"/>
+      <c r="C79" s="0" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="0" t="s">
-        <v>164</v>
-      </c>
-      <c r="B76" s="2"/>
-      <c r="C76" s="0" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="0" t="s">
-        <v>166</v>
-      </c>
-      <c r="B77" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="C77" s="0" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B78" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="C78" s="0" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B79" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="C79" s="0" t="s">
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="0" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B80" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="B80" s="2"/>
       <c r="C80" s="0" t="s">
-        <v>35</v>
+        <v>173</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="0" t="s">
+        <v>174</v>
+      </c>
       <c r="B81" s="2" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B82" s="2" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B83" s="2" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C83" s="0" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B84" s="2" t="s">
-        <v>179</v>
+        <v>34</v>
       </c>
       <c r="C84" s="0" t="s">
-        <v>180</v>
+        <v>35</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1978,41 +2002,41 @@
       </c>
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="0" t="s">
+      <c r="B112" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="B112" s="2" t="s">
+      <c r="C112" s="0" t="s">
         <v>236</v>
-      </c>
-      <c r="C112" s="0" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B113" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="C113" s="0" t="s">
         <v>238</v>
-      </c>
-      <c r="C113" s="0" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B114" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="C114" s="0" t="s">
         <v>240</v>
-      </c>
-      <c r="C114" s="0" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B115" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="C115" s="0" t="s">
         <v>242</v>
       </c>
-      <c r="C115" s="0" t="s">
+    </row>
+    <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="0" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B116" s="2" t="s">
         <v>244</v>
       </c>
@@ -2046,42 +2070,39 @@
     </row>
     <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B120" s="2" t="s">
-        <v>99</v>
+        <v>252</v>
       </c>
       <c r="C120" s="0" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B121" s="2" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C121" s="0" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B122" s="2" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C122" s="0" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B123" s="2" t="s">
-        <v>108</v>
+        <v>258</v>
       </c>
       <c r="C123" s="0" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="0" t="s">
-        <v>258</v>
-      </c>
       <c r="B124" s="2" t="s">
-        <v>259</v>
+        <v>99</v>
       </c>
       <c r="C124" s="0" t="s">
         <v>260</v>
@@ -2089,26 +2110,61 @@
     </row>
     <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B125" s="2" t="s">
-        <v>34</v>
+        <v>261</v>
       </c>
       <c r="C125" s="0" t="s">
-        <v>35</v>
+        <v>262</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B126" s="2" t="s">
-        <v>36</v>
+        <v>263</v>
       </c>
       <c r="C126" s="0" t="s">
-        <v>149</v>
+        <v>264</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B127" s="2" t="s">
-        <v>261</v>
+        <v>108</v>
       </c>
       <c r="C127" s="0" t="s">
-        <v>262</v>
+        <v>265</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="0" t="s">
+        <v>266</v>
+      </c>
+      <c r="B128" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="C128" s="0" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B129" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C129" s="0" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B130" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C130" s="0" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B131" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="C131" s="0" t="s">
+        <v>270</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- adds `{WEIGHTin}` placeholder substitude by the current batch size (g) in command actions - adds "Load p-i-d from background" setting to configure the PID to the settings stored in background profile
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/eventsliders.xlsx
+++ b/doc/help_dialogs/Input_files/eventsliders.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sliders" sheetId="1" state="visible" r:id="rId2"/>
@@ -98,7 +98,7 @@
     <t xml:space="preserve">tn:Note: "{}" can be used as a placeholder, it will be substituted by (value*factor + offset). In all slider command actions, but for IO, VOUT, S7 and RC Commands, the bound value is converted from a float to an int.\n</t>
   </si>
   <si>
-    <t xml:space="preserve">tn:Note: The placeholders {ET}, {BT}, {time}, {ETB}, {BTB} will be substituted by the current ET, BT, time, ET background, BT background value in Serial/CallProgram/MODBUS/S7/WebSocket commands\n</t>
+    <t xml:space="preserve">tn:Note: The placeholders {ET}, {BT}, {time}, {ETB}, {BTB}, and {WEIGHTin} will be substituted by the current ET, BT, time, ET background, BT background value, and batch size (in g) in Serial/Artisan/CallProgram/MODBUS/S7/WebSocket commands\n</t>
   </si>
   <si>
     <t xml:space="preserve">tn:Note: commands can be sequenced, separated by semicolons like in “&lt;cmd1&gt;;&lt;cmd2&gt;;&lt;cmd3&gt;”\n</t>
@@ -969,11 +969,11 @@
   </sheetPr>
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.03125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="70.31"/>
@@ -1090,13 +1090,13 @@
   </sheetPr>
   <dimension ref="A1:C133"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.03125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.57"/>
   </cols>
   <sheetData>

</xml_diff>